<commit_message>
pandas finish and 7 opencv commit
</commit_message>
<xml_diff>
--- a/파이썬의도구들/CH3_파이썬의도구들_라이브러리/6_pandas/학생리스트.xlsx
+++ b/파이썬의도구들/CH3_파이썬의도구들_라이브러리/6_pandas/학생리스트.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\thate\PycharmProjects\python_tools\파이썬의도구들\CH3_파이썬의도구들_라이브러리\6_pandas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84089F72-3038-47D6-94C8-4D4D7E9FBB3E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{317A06B6-02E5-4F7C-96B8-4A600F014684}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -376,7 +376,7 @@
   <dimension ref="B2:D7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="L9" sqref="L9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>

</xml_diff>